<commit_message>
Updating the daily scores
</commit_message>
<xml_diff>
--- a/data/Firmen/creators/2025-02-01/Daily_Motivations.xlsx
+++ b/data/Firmen/creators/2025-02-01/Daily_Motivations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -779,6 +779,114 @@
         <v>0</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>sleep</t>
+        </is>
+      </c>
+      <c r="C20" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2025-02-07</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>weekly_activity</t>
+        </is>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2025-02-08</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>sleep</t>
+        </is>
+      </c>
+      <c r="C23" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2025-02-08</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2025-02-08</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>weekly_activity</t>
+        </is>
+      </c>
+      <c r="C25" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating Baselines and Daily Scores
</commit_message>
<xml_diff>
--- a/data/Firmen/creators/2025-02-01/Daily_Motivations.xlsx
+++ b/data/Firmen/creators/2025-02-01/Daily_Motivations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -941,6 +941,60 @@
         <v>0</v>
       </c>
     </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>2025-02-10</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>sleep</t>
+        </is>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>2025-02-10</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C30" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>2025-02-10</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>weekly_activity</t>
+        </is>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Update the daily Scores
</commit_message>
<xml_diff>
--- a/data/Firmen/creators/2025-02-01/Daily_Motivations.xlsx
+++ b/data/Firmen/creators/2025-02-01/Daily_Motivations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1103,6 +1103,60 @@
         <v>0</v>
       </c>
     </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>2025-02-13</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>sleep</t>
+        </is>
+      </c>
+      <c r="C38" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>2025-02-13</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C39" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>2025-02-13</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>weekly_activity</t>
+        </is>
+      </c>
+      <c r="C40" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the Daily Scores - New baseline
</commit_message>
<xml_diff>
--- a/data/Firmen/creators/2025-02-01/Daily_Motivations.xlsx
+++ b/data/Firmen/creators/2025-02-01/Daily_Motivations.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1157,6 +1157,222 @@
         <v>0</v>
       </c>
     </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>2025-02-14</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>sleep</t>
+        </is>
+      </c>
+      <c r="C41" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>2025-02-14</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C42" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>2025-02-14</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>weekly_activity</t>
+        </is>
+      </c>
+      <c r="C43" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>2025-02-15</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>sleep</t>
+        </is>
+      </c>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>2025-02-15</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>2025-02-15</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>weekly_activity</t>
+        </is>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>2025-02-16</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>sleep</t>
+        </is>
+      </c>
+      <c r="C47" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>2025-02-16</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C48" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>2025-02-16</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>weekly_activity</t>
+        </is>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>2025-02-17</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>sleep</t>
+        </is>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>2025-02-17</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>activity</t>
+        </is>
+      </c>
+      <c r="C51" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>2025-02-17</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>weekly_activity</t>
+        </is>
+      </c>
+      <c r="C52" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>